<commit_message>
Additional updates to leveraging spreadsheet on Google.
</commit_message>
<xml_diff>
--- a/data/TBEP_Funding_Sources_2016-2018_v20190107.xlsx
+++ b/data/TBEP_Funding_Sources_2016-2018_v20190107.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\rprojects\TBEP_Funding\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D40D07-AA6B-4B91-93A4-0E862E8BFFD5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F514AF7E-495E-46AD-9999-C2F37E47D54C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18660" windowHeight="9600" activeTab="4" xr2:uid="{FA6988C6-5DA2-46AD-A097-2C9F9922665D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18660" windowHeight="9600" xr2:uid="{FA6988C6-5DA2-46AD-A097-2C9F9922665D}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="35">
   <si>
     <t>City Cash</t>
   </si>
@@ -133,6 +133,12 @@
   </si>
   <si>
     <t>Pasco Co.</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Leveraging</t>
   </si>
 </sst>
 </file>
@@ -252,7 +258,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -292,6 +298,10 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -972,7 +982,7 @@
                   <c:v>1616909</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>147579</c:v>
+                  <c:v>1553462</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>1903000</c:v>
@@ -1825,7 +1835,7 @@
                   <c:v>1616909</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>147579</c:v>
+                  <c:v>1553462</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>1903000</c:v>
@@ -2398,6 +2408,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001D-1272-4CF4-89F5-4D4594C02A38}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:dLbl>
@@ -2661,7 +2676,7 @@
                   <c:v>1616909</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>147579</c:v>
+                  <c:v>1553462</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>1903000</c:v>
@@ -3514,7 +3529,7 @@
                   <c:v>1616909</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>147579</c:v>
+                  <c:v>1553462</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>1903000</c:v>
@@ -4165,7 +4180,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="-3.8925800941548974E-2"/>
-                  <c:y val="2.0420715703220023E-2"/>
+                  <c:y val="3.0176813264195516E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="bestFit"/>
@@ -4355,7 +4370,7 @@
                   <c:v>1616909</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>147579</c:v>
+                  <c:v>1553462</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>1903000</c:v>
@@ -5006,7 +5021,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="-3.8925800941548974E-2"/>
-                  <c:y val="2.0420715703220023E-2"/>
+                  <c:y val="3.0176813264195516E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="bestFit"/>
@@ -5196,7 +5211,7 @@
                   <c:v>1616909</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>147579</c:v>
+                  <c:v>1553462</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>1903000</c:v>
@@ -6037,7 +6052,7 @@
                   <c:v>1616909</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>147579</c:v>
+                  <c:v>1553462</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>1903000</c:v>
@@ -6687,8 +6702,8 @@
               <c:idx val="5"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-2.8583593717452064E-2"/>
-                  <c:y val="4.6445169963510655E-3"/>
+                  <c:x val="-3.4932800066658415E-2"/>
+                  <c:y val="1.7652647077651878E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -6890,7 +6905,7 @@
                   <c:v>1616909</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>147579</c:v>
+                  <c:v>1553462</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>1903000</c:v>
@@ -7731,7 +7746,7 @@
                   <c:v>1616909</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>147579</c:v>
+                  <c:v>1553462</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>1903000</c:v>
@@ -8572,7 +8587,7 @@
                   <c:v>1616909</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>147579</c:v>
+                  <c:v>1553462</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>1903000</c:v>
@@ -14404,8 +14419,8 @@
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>171336</xdr:rowOff>
     </xdr:to>
@@ -14423,7 +14438,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4229100" y="4152900"/>
-          <a:ext cx="3733800" cy="342786"/>
+          <a:ext cx="4076700" cy="342786"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14456,7 +14471,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>$14.81</a:t>
+            <a:t>$16.21</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1600" baseline="0">
@@ -14472,7 +14487,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>$8</a:t>
+            <a:t>$8.52</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1600" baseline="0">
@@ -14654,7 +14669,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>$14.81</a:t>
+            <a:t>$16.21</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1600" baseline="0">
@@ -14670,7 +14685,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>$298</a:t>
+            <a:t>$326</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1600" baseline="0">
@@ -14852,7 +14867,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>$14.81</a:t>
+            <a:t>$16.21</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1600" baseline="0">
@@ -14868,7 +14883,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>$34</a:t>
+            <a:t>$37</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1600" baseline="0">
@@ -15050,7 +15065,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>$14.81</a:t>
+            <a:t>$16.21</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1600" baseline="0">
@@ -15066,7 +15081,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>$494</a:t>
+            <a:t>$540</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1600" baseline="0">
@@ -15248,7 +15263,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>$14.81</a:t>
+            <a:t>$16.21</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1600" baseline="0">
@@ -15264,7 +15279,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>$56</a:t>
+            <a:t>$61</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1600" baseline="0">
@@ -15446,7 +15461,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>$14.81</a:t>
+            <a:t>$16.21</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1600" baseline="0">
@@ -15462,7 +15477,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>$56</a:t>
+            <a:t>$61</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1600" baseline="0">
@@ -15644,7 +15659,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>$14.81</a:t>
+            <a:t>$16.21</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1600" baseline="0">
@@ -15660,7 +15675,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>$129</a:t>
+            <a:t>$141</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1600" baseline="0">
@@ -15842,7 +15857,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>$14.81</a:t>
+            <a:t>$16.21</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1600" baseline="0">
@@ -15858,7 +15873,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>$190</a:t>
+            <a:t>$208</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1600" baseline="0">
@@ -16040,7 +16055,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>$14.81</a:t>
+            <a:t>$16.21</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1600" baseline="0">
@@ -16056,7 +16071,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>$138</a:t>
+            <a:t>$151</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1600" baseline="0">
@@ -16238,7 +16253,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>$14.81</a:t>
+            <a:t>$16.21</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1600" baseline="0">
@@ -16254,7 +16269,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>$106</a:t>
+            <a:t>$116</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1600" baseline="0">
@@ -16576,8 +16591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A1E8E95-0C1B-4D52-B379-1283BC2041C5}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16597,8 +16612,8 @@
         <v>8</v>
       </c>
       <c r="D1" s="3">
-        <f>(B1/$B$15)</f>
-        <v>1.8151257303119332E-2</v>
+        <f t="shared" ref="D1:D14" si="0">(B1/$B$15)</f>
+        <v>1.6577185031186697E-2</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -16612,8 +16627,8 @@
         <v>9</v>
       </c>
       <c r="D2" s="3">
-        <f>(B2/$B$15)</f>
-        <v>3.5309431874750878E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.2247407204857179E-2</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -16627,8 +16642,8 @@
         <v>10</v>
       </c>
       <c r="D3" s="3">
-        <f>(B3/$B$15)</f>
-        <v>1.3147176670893693E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.200705695872935E-2</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -16642,8 +16657,8 @@
         <v>0</v>
       </c>
       <c r="D4" s="3">
-        <f>(B4/$B$15)</f>
-        <v>4.5613657216019017E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.1658052827509985E-2</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -16657,8 +16672,8 @@
         <v>1</v>
       </c>
       <c r="D5" s="3">
-        <f>(B5/$B$15)</f>
-        <v>0.18266346429820809</v>
+        <f t="shared" si="0"/>
+        <v>0.16682293659010525</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -16672,8 +16687,8 @@
         <v>2</v>
       </c>
       <c r="D6" s="3">
-        <f>(B6/$B$15)</f>
-        <v>0.10591360555086204</v>
+        <f t="shared" si="0"/>
+        <v>9.672880546049191E-2</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -16687,8 +16702,8 @@
         <v>3</v>
       </c>
       <c r="D7" s="3">
-        <f>(B7/$B$15)</f>
-        <v>3.8492922744768961E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.5154826581712907E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -16702,8 +16717,8 @@
         <v>11</v>
       </c>
       <c r="D8" s="3">
-        <f>(B8/$B$15)</f>
-        <v>0.12009408536107846</v>
+        <f t="shared" si="0"/>
+        <v>0.10967955778135549</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -16717,8 +16732,8 @@
         <v>12</v>
       </c>
       <c r="D9" s="3">
-        <f>(B9/$B$15)</f>
-        <v>0.11695108506116457</v>
+        <f t="shared" si="0"/>
+        <v>0.1068091176429859</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -16732,8 +16747,8 @@
         <v>14</v>
       </c>
       <c r="D10" s="3">
-        <f>(B10/$B$15)</f>
-        <v>4.3968909320811045E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.0155937038328163E-2</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -16747,8 +16762,8 @@
         <v>15</v>
       </c>
       <c r="D11" s="3">
-        <f>(B11/$B$15)</f>
-        <v>3.1990184464433524E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.92160040592656E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -16762,8 +16777,8 @@
         <v>5</v>
       </c>
       <c r="D12" s="3">
-        <f>(B12/$B$15)</f>
-        <v>0.10920695115361484</v>
+        <f t="shared" si="0"/>
+        <v>9.9736552996476421E-2</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -16771,14 +16786,14 @@
         <v>7</v>
       </c>
       <c r="B13" s="2">
-        <v>147579</v>
+        <v>1553462</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D13" s="3">
-        <f>(B13/$B$15)</f>
-        <v>9.9675693834961176E-3</v>
+        <f t="shared" si="0"/>
+        <v>9.5822922063648758E-2</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -16792,14 +16807,26 @@
         <v>6</v>
       </c>
       <c r="D14" s="3">
-        <f>(B14/$B$15)</f>
-        <v>0.12852969959677943</v>
+        <f t="shared" si="0"/>
+        <v>0.11738363776334639</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15">
+      <c r="A15" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="14">
         <f>SUM(B1:B14)</f>
-        <v>14805916.5</v>
+        <v>16211799.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="16">
+        <f>B15/B14</f>
+        <v>8.5190748817656328</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -16967,12 +16994,13 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+      <selection activeCell="A16" sqref="A16:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -16987,8 +17015,8 @@
         <v>8</v>
       </c>
       <c r="D1" s="3">
-        <f>(B1/$B$16)</f>
-        <v>1.8151257303119332E-2</v>
+        <f t="shared" ref="D1:D15" si="0">(B1/$B$16)</f>
+        <v>1.6577185031186697E-2</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17002,8 +17030,8 @@
         <v>9</v>
       </c>
       <c r="D2" s="3">
-        <f>(B2/$B$16)</f>
-        <v>3.5309431874750878E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.2247407204857179E-2</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17017,8 +17045,8 @@
         <v>10</v>
       </c>
       <c r="D3" s="3">
-        <f>(B3/$B$16)</f>
-        <v>1.3147176670893693E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.200705695872935E-2</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17030,8 +17058,8 @@
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="3">
-        <f>(B4/$B$16)</f>
-        <v>3.3580494662387161E-3</v>
+        <f t="shared" si="0"/>
+        <v>3.0668402974019016E-3</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17046,8 +17074,8 @@
         <v>0</v>
       </c>
       <c r="D5" s="3">
-        <f>(B5/$B$16)</f>
-        <v>4.2255607749780301E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.8591212530108089E-2</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17061,8 +17089,8 @@
         <v>1</v>
       </c>
       <c r="D6" s="3">
-        <f>(B6/$B$16)</f>
-        <v>0.18266346429820809</v>
+        <f t="shared" si="0"/>
+        <v>0.16682293659010525</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17076,8 +17104,8 @@
         <v>2</v>
       </c>
       <c r="D7" s="3">
-        <f>(B7/$B$16)</f>
-        <v>0.10591360555086204</v>
+        <f t="shared" si="0"/>
+        <v>9.672880546049191E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17091,8 +17119,8 @@
         <v>3</v>
       </c>
       <c r="D8" s="3">
-        <f>(B8/$B$16)</f>
-        <v>3.8492922744768961E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.5154826581712907E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17106,8 +17134,8 @@
         <v>11</v>
       </c>
       <c r="D9" s="3">
-        <f>(B9/$B$16)</f>
-        <v>0.12009408536107846</v>
+        <f t="shared" si="0"/>
+        <v>0.10967955778135549</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17121,8 +17149,8 @@
         <v>12</v>
       </c>
       <c r="D10" s="3">
-        <f>(B10/$B$16)</f>
-        <v>0.11695108506116457</v>
+        <f t="shared" si="0"/>
+        <v>0.1068091176429859</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17136,8 +17164,8 @@
         <v>14</v>
       </c>
       <c r="D11" s="3">
-        <f>(B11/$B$16)</f>
-        <v>4.3968909320811045E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.0155937038328163E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17151,8 +17179,8 @@
         <v>15</v>
       </c>
       <c r="D12" s="3">
-        <f>(B12/$B$16)</f>
-        <v>3.1990184464433524E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.92160040592656E-2</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17166,8 +17194,8 @@
         <v>5</v>
       </c>
       <c r="D13" s="3">
-        <f>(B13/$B$16)</f>
-        <v>0.10920695115361484</v>
+        <f t="shared" si="0"/>
+        <v>9.9736552996476421E-2</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17175,14 +17203,14 @@
         <v>7</v>
       </c>
       <c r="B14" s="2">
-        <v>147579</v>
+        <v>1553462</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="3">
-        <f>(B14/$B$16)</f>
-        <v>9.9675693834961176E-3</v>
+        <f t="shared" si="0"/>
+        <v>9.5822922063648758E-2</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17196,14 +17224,26 @@
         <v>6</v>
       </c>
       <c r="D15" s="3">
-        <f>(B15/$B$16)</f>
-        <v>0.12852969959677943</v>
+        <f t="shared" si="0"/>
+        <v>0.11738363776334639</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>33</v>
+      </c>
       <c r="B16" s="14">
         <f>SUM(B1:B15)</f>
-        <v>14805916.5</v>
+        <v>16211799.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="16">
+        <f>B16/B4</f>
+        <v>326.06849494157166</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -17373,7 +17413,7 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17393,8 +17433,8 @@
         <v>8</v>
       </c>
       <c r="D1" s="3">
-        <f>(B1/$B$16)</f>
-        <v>1.8151257303119332E-2</v>
+        <f t="shared" ref="D1:D15" si="0">(B1/$B$16)</f>
+        <v>1.6577185031186697E-2</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17408,8 +17448,8 @@
         <v>9</v>
       </c>
       <c r="D2" s="3">
-        <f>(B2/$B$16)</f>
-        <v>3.5309431874750878E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.2247407204857179E-2</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17423,8 +17463,8 @@
         <v>10</v>
       </c>
       <c r="D3" s="3">
-        <f>(B3/$B$16)</f>
-        <v>1.3147176670893693E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.200705695872935E-2</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17438,8 +17478,8 @@
         <v>0</v>
       </c>
       <c r="D4" s="3">
-        <f>(B4/$B$16)</f>
-        <v>4.5613657216019017E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.1658052827509985E-2</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17453,8 +17493,8 @@
         <v>1</v>
       </c>
       <c r="D5" s="3">
-        <f>(B5/$B$16)</f>
-        <v>0.18266346429820809</v>
+        <f t="shared" si="0"/>
+        <v>0.16682293659010525</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17468,8 +17508,8 @@
         <v>2</v>
       </c>
       <c r="D6" s="3">
-        <f>(B6/$B$16)</f>
-        <v>0.10591360555086204</v>
+        <f t="shared" si="0"/>
+        <v>9.672880546049191E-2</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17483,8 +17523,8 @@
         <v>3</v>
       </c>
       <c r="D7" s="3">
-        <f>(B7/$B$16)</f>
-        <v>3.8492922744768961E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.5154826581712907E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17496,8 +17536,8 @@
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="3">
-        <f>(B8/$B$16)</f>
-        <v>2.9454644026933423E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.6900345023388676E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17512,8 +17552,8 @@
         <v>11</v>
       </c>
       <c r="D9" s="3">
-        <f>(B9/$B$16)</f>
-        <v>9.0639441334145032E-2</v>
+        <f t="shared" si="0"/>
+        <v>8.2779212757966819E-2</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17527,8 +17567,8 @@
         <v>12</v>
       </c>
       <c r="D10" s="3">
-        <f>(B10/$B$16)</f>
-        <v>0.11695108506116457</v>
+        <f t="shared" si="0"/>
+        <v>0.1068091176429859</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17542,8 +17582,8 @@
         <v>14</v>
       </c>
       <c r="D11" s="3">
-        <f>(B11/$B$16)</f>
-        <v>4.3968909320811045E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.0155937038328163E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17557,8 +17597,8 @@
         <v>15</v>
       </c>
       <c r="D12" s="3">
-        <f>(B12/$B$16)</f>
-        <v>3.1990184464433524E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.92160040592656E-2</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17572,8 +17612,8 @@
         <v>5</v>
       </c>
       <c r="D13" s="3">
-        <f>(B13/$B$16)</f>
-        <v>0.10920695115361484</v>
+        <f t="shared" si="0"/>
+        <v>9.9736552996476421E-2</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17581,14 +17621,14 @@
         <v>7</v>
       </c>
       <c r="B14" s="2">
-        <v>147579</v>
+        <v>1553462</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="3">
-        <f>(B14/$B$16)</f>
-        <v>9.9675693834961176E-3</v>
+        <f t="shared" si="0"/>
+        <v>9.5822922063648758E-2</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17602,14 +17642,26 @@
         <v>6</v>
       </c>
       <c r="D15" s="3">
-        <f>(B15/$B$16)</f>
-        <v>0.12852969959677943</v>
+        <f t="shared" si="0"/>
+        <v>0.11738363776334639</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>33</v>
+      </c>
       <c r="B16" s="14">
         <f>SUM(B1:B15)</f>
-        <v>14805916.5</v>
+        <v>16211799.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="16">
+        <f>B16/B8</f>
+        <v>37.174244387220448</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -17779,7 +17831,7 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+      <selection activeCell="A16" sqref="A16:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17799,8 +17851,8 @@
         <v>8</v>
       </c>
       <c r="D1" s="3">
-        <f>(B1/$B$16)</f>
-        <v>1.8151257303119332E-2</v>
+        <f t="shared" ref="D1:D15" si="0">(B1/$B$16)</f>
+        <v>1.6577185031186697E-2</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17814,8 +17866,8 @@
         <v>9</v>
       </c>
       <c r="D2" s="3">
-        <f>(B2/$B$16)</f>
-        <v>3.5309431874750878E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.2247407204857179E-2</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17829,8 +17881,8 @@
         <v>10</v>
       </c>
       <c r="D3" s="3">
-        <f>(B3/$B$16)</f>
-        <v>1.3147176670893693E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.200705695872935E-2</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17844,8 +17896,8 @@
         <v>0</v>
       </c>
       <c r="D4" s="3">
-        <f>(B4/$B$16)</f>
-        <v>4.5613657216019017E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.1658052827509985E-2</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17859,8 +17911,8 @@
         <v>1</v>
       </c>
       <c r="D5" s="3">
-        <f>(B5/$B$16)</f>
-        <v>0.18266346429820809</v>
+        <f t="shared" si="0"/>
+        <v>0.16682293659010525</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17874,8 +17926,8 @@
         <v>2</v>
       </c>
       <c r="D6" s="3">
-        <f>(B6/$B$16)</f>
-        <v>0.10591360555086204</v>
+        <f t="shared" si="0"/>
+        <v>9.672880546049191E-2</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17889,8 +17941,8 @@
         <v>3</v>
       </c>
       <c r="D7" s="3">
-        <f>(B7/$B$16)</f>
-        <v>3.8492922744768961E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.5154826581712907E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17902,8 +17954,8 @@
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="3">
-        <f>(B8/$B$16)</f>
-        <v>2.0262170193922138E-3</v>
+        <f t="shared" si="0"/>
+        <v>1.8505040109828646E-3</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17918,8 +17970,8 @@
         <v>11</v>
       </c>
       <c r="D9" s="3">
-        <f>(B9/$B$16)</f>
-        <v>0.11806786834168624</v>
+        <f t="shared" si="0"/>
+        <v>0.10782905377037262</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17933,8 +17985,8 @@
         <v>12</v>
       </c>
       <c r="D10" s="3">
-        <f>(B10/$B$16)</f>
-        <v>0.11695108506116457</v>
+        <f t="shared" si="0"/>
+        <v>0.1068091176429859</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17948,8 +18000,8 @@
         <v>14</v>
       </c>
       <c r="D11" s="3">
-        <f>(B11/$B$16)</f>
-        <v>4.3968909320811045E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.0155937038328163E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17963,8 +18015,8 @@
         <v>15</v>
       </c>
       <c r="D12" s="3">
-        <f>(B12/$B$16)</f>
-        <v>3.1990184464433524E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.92160040592656E-2</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17978,8 +18030,8 @@
         <v>5</v>
       </c>
       <c r="D13" s="3">
-        <f>(B13/$B$16)</f>
-        <v>0.10920695115361484</v>
+        <f t="shared" si="0"/>
+        <v>9.9736552996476421E-2</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17987,14 +18039,14 @@
         <v>7</v>
       </c>
       <c r="B14" s="2">
-        <v>147579</v>
+        <v>1553462</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="3">
-        <f>(B14/$B$16)</f>
-        <v>9.9675693834961176E-3</v>
+        <f t="shared" si="0"/>
+        <v>9.5822922063648758E-2</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18008,14 +18060,26 @@
         <v>6</v>
       </c>
       <c r="D15" s="3">
-        <f>(B15/$B$16)</f>
-        <v>0.12852969959677943</v>
+        <f t="shared" si="0"/>
+        <v>0.11738363776334639</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>33</v>
+      </c>
       <c r="B16" s="14">
         <f>SUM(B1:B15)</f>
-        <v>14805916.5</v>
+        <v>16211799.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="16">
+        <f>B16/B8</f>
+        <v>540.39331666666669</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -18185,7 +18249,7 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18205,8 +18269,8 @@
         <v>8</v>
       </c>
       <c r="D1" s="3">
-        <f>(B1/$B$16)</f>
-        <v>1.8151257303119332E-2</v>
+        <f t="shared" ref="D1:D15" si="0">(B1/$B$16)</f>
+        <v>1.6577185031186697E-2</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18220,8 +18284,8 @@
         <v>9</v>
       </c>
       <c r="D2" s="3">
-        <f>(B2/$B$16)</f>
-        <v>3.5309431874750878E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.2247407204857179E-2</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18235,8 +18299,8 @@
         <v>10</v>
       </c>
       <c r="D3" s="3">
-        <f>(B3/$B$16)</f>
-        <v>1.3147176670893693E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.200705695872935E-2</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18250,8 +18314,8 @@
         <v>0</v>
       </c>
       <c r="D4" s="3">
-        <f>(B4/$B$16)</f>
-        <v>4.5613657216019017E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.1658052827509985E-2</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18265,8 +18329,8 @@
         <v>1</v>
       </c>
       <c r="D5" s="3">
-        <f>(B5/$B$16)</f>
-        <v>0.18266346429820809</v>
+        <f t="shared" si="0"/>
+        <v>0.16682293659010525</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18278,8 +18342,8 @@
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="3">
-        <f>(B6/$B$16)</f>
-        <v>1.7879946844222713E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.6329402544116092E-2</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18294,8 +18358,8 @@
         <v>2</v>
       </c>
       <c r="D7" s="3">
-        <f>(B7/$B$16)</f>
-        <v>8.8033658706639331E-2</v>
+        <f t="shared" si="0"/>
+        <v>8.0399402916375817E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18309,8 +18373,8 @@
         <v>3</v>
       </c>
       <c r="D8" s="3">
-        <f>(B8/$B$16)</f>
-        <v>3.8492922744768961E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.5154826581712907E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18324,8 +18388,8 @@
         <v>11</v>
       </c>
       <c r="D9" s="3">
-        <f>(B9/$B$16)</f>
-        <v>0.12009408536107846</v>
+        <f t="shared" si="0"/>
+        <v>0.10967955778135549</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18339,8 +18403,8 @@
         <v>12</v>
       </c>
       <c r="D10" s="3">
-        <f>(B10/$B$16)</f>
-        <v>0.11695108506116457</v>
+        <f t="shared" si="0"/>
+        <v>0.1068091176429859</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18354,8 +18418,8 @@
         <v>14</v>
       </c>
       <c r="D11" s="3">
-        <f>(B11/$B$16)</f>
-        <v>4.3968909320811045E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.0155937038328163E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18369,8 +18433,8 @@
         <v>15</v>
       </c>
       <c r="D12" s="3">
-        <f>(B12/$B$16)</f>
-        <v>3.1990184464433524E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.92160040592656E-2</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18384,8 +18448,8 @@
         <v>5</v>
       </c>
       <c r="D13" s="3">
-        <f>(B13/$B$16)</f>
-        <v>0.10920695115361484</v>
+        <f t="shared" si="0"/>
+        <v>9.9736552996476421E-2</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18393,14 +18457,14 @@
         <v>7</v>
       </c>
       <c r="B14" s="2">
-        <v>147579</v>
+        <v>1553462</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="3">
-        <f>(B14/$B$16)</f>
-        <v>9.9675693834961176E-3</v>
+        <f t="shared" si="0"/>
+        <v>9.5822922063648758E-2</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18414,14 +18478,26 @@
         <v>6</v>
       </c>
       <c r="D15" s="3">
-        <f>(B15/$B$16)</f>
-        <v>0.12852969959677943</v>
+        <f t="shared" si="0"/>
+        <v>0.11738363776334639</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>33</v>
+      </c>
       <c r="B16" s="14">
         <f>SUM(B1:B15)</f>
-        <v>14805916.5</v>
+        <v>16211799.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="16">
+        <f>B16/B6</f>
+        <v>61.239227663006318</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -18590,8 +18666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EAB5668-FE4B-42A2-8C10-8072D130CE6B}">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18611,8 +18687,8 @@
         <v>8</v>
       </c>
       <c r="D1" s="3">
-        <f>(B1/$B$16)</f>
-        <v>1.8151257303119332E-2</v>
+        <f t="shared" ref="D1:D15" si="0">(B1/$B$16)</f>
+        <v>1.6577185031186697E-2</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18626,8 +18702,8 @@
         <v>9</v>
       </c>
       <c r="D2" s="3">
-        <f>(B2/$B$16)</f>
-        <v>3.5309431874750878E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.2247407204857179E-2</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18641,8 +18717,8 @@
         <v>10</v>
       </c>
       <c r="D3" s="3">
-        <f>(B3/$B$16)</f>
-        <v>1.3147176670893693E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.200705695872935E-2</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18656,8 +18732,8 @@
         <v>0</v>
       </c>
       <c r="D4" s="3">
-        <f>(B4/$B$16)</f>
-        <v>4.5613657216019017E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.1658052827509985E-2</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18671,8 +18747,8 @@
         <v>1</v>
       </c>
       <c r="D5" s="3">
-        <f>(B5/$B$16)</f>
-        <v>0.18266346429820809</v>
+        <f t="shared" si="0"/>
+        <v>0.16682293659010525</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18684,8 +18760,8 @@
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="3">
-        <f>(B6/$B$16)</f>
-        <v>1.7879946844222713E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.6329402544116092E-2</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18700,8 +18776,8 @@
         <v>2</v>
       </c>
       <c r="D7" s="3">
-        <f>(B7/$B$16)</f>
-        <v>8.8033658706639331E-2</v>
+        <f t="shared" si="0"/>
+        <v>8.0399402916375817E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18715,8 +18791,8 @@
         <v>3</v>
       </c>
       <c r="D8" s="3">
-        <f>(B8/$B$16)</f>
-        <v>3.8492922744768961E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.5154826581712907E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18730,8 +18806,8 @@
         <v>11</v>
       </c>
       <c r="D9" s="3">
-        <f>(B9/$B$16)</f>
-        <v>0.12009408536107846</v>
+        <f t="shared" si="0"/>
+        <v>0.10967955778135549</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18745,8 +18821,8 @@
         <v>12</v>
       </c>
       <c r="D10" s="3">
-        <f>(B10/$B$16)</f>
-        <v>0.11695108506116457</v>
+        <f t="shared" si="0"/>
+        <v>0.1068091176429859</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18760,8 +18836,8 @@
         <v>14</v>
       </c>
       <c r="D11" s="3">
-        <f>(B11/$B$16)</f>
-        <v>4.3968909320811045E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.0155937038328163E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18775,8 +18851,8 @@
         <v>15</v>
       </c>
       <c r="D12" s="3">
-        <f>(B12/$B$16)</f>
-        <v>3.1990184464433524E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.92160040592656E-2</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18790,8 +18866,8 @@
         <v>5</v>
       </c>
       <c r="D13" s="3">
-        <f>(B13/$B$16)</f>
-        <v>0.10920695115361484</v>
+        <f t="shared" si="0"/>
+        <v>9.9736552996476421E-2</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18799,14 +18875,14 @@
         <v>7</v>
       </c>
       <c r="B14" s="2">
-        <v>147579</v>
+        <v>1553462</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="3">
-        <f>(B14/$B$16)</f>
-        <v>9.9675693834961176E-3</v>
+        <f t="shared" si="0"/>
+        <v>9.5822922063648758E-2</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18820,14 +18896,26 @@
         <v>6</v>
       </c>
       <c r="D15" s="3">
-        <f>(B15/$B$16)</f>
-        <v>0.12852969959677943</v>
+        <f t="shared" si="0"/>
+        <v>0.11738363776334639</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>33</v>
+      </c>
       <c r="B16" s="14">
         <f>SUM(B1:B15)</f>
-        <v>14805916.5</v>
+        <v>16211799.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="16">
+        <f>B16/B6</f>
+        <v>61.239227663006318</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -18997,7 +19085,7 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19017,8 +19105,8 @@
         <v>8</v>
       </c>
       <c r="D1" s="3">
-        <f>(B1/$B$16)</f>
-        <v>1.8151257303119332E-2</v>
+        <f t="shared" ref="D1:D15" si="0">(B1/$B$16)</f>
+        <v>1.6577185031186697E-2</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19032,8 +19120,8 @@
         <v>9</v>
       </c>
       <c r="D2" s="3">
-        <f>(B2/$B$16)</f>
-        <v>3.5309431874750878E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.2247407204857179E-2</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19047,8 +19135,8 @@
         <v>10</v>
       </c>
       <c r="D3" s="3">
-        <f>(B3/$B$16)</f>
-        <v>1.3147176670893693E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.200705695872935E-2</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19062,8 +19150,8 @@
         <v>0</v>
       </c>
       <c r="D4" s="3">
-        <f>(B4/$B$16)</f>
-        <v>4.5613657216019017E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.1658052827509985E-2</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19077,8 +19165,8 @@
         <v>1</v>
       </c>
       <c r="D5" s="3">
-        <f>(B5/$B$16)</f>
-        <v>0.18266346429820809</v>
+        <f t="shared" si="0"/>
+        <v>0.16682293659010525</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19090,8 +19178,8 @@
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="3">
-        <f>(B6/$B$16)</f>
-        <v>7.7391359055685614E-3</v>
+        <f t="shared" si="0"/>
+        <v>7.0680000699490514E-3</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19106,8 +19194,8 @@
         <v>2</v>
       </c>
       <c r="D7" s="3">
-        <f>(B7/$B$16)</f>
-        <v>9.8174469645293486E-2</v>
+        <f t="shared" si="0"/>
+        <v>8.9660805390542858E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19121,8 +19209,8 @@
         <v>3</v>
       </c>
       <c r="D8" s="3">
-        <f>(B8/$B$16)</f>
-        <v>3.8492922744768961E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.5154826581712907E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19136,8 +19224,8 @@
         <v>11</v>
       </c>
       <c r="D9" s="3">
-        <f>(B9/$B$16)</f>
-        <v>0.12009408536107846</v>
+        <f t="shared" si="0"/>
+        <v>0.10967955778135549</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19151,8 +19239,8 @@
         <v>12</v>
       </c>
       <c r="D10" s="3">
-        <f>(B10/$B$16)</f>
-        <v>0.11695108506116457</v>
+        <f t="shared" si="0"/>
+        <v>0.1068091176429859</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19166,8 +19254,8 @@
         <v>14</v>
       </c>
       <c r="D11" s="3">
-        <f>(B11/$B$16)</f>
-        <v>4.3968909320811045E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.0155937038328163E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19181,8 +19269,8 @@
         <v>15</v>
       </c>
       <c r="D12" s="3">
-        <f>(B12/$B$16)</f>
-        <v>3.1990184464433524E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.92160040592656E-2</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19196,8 +19284,8 @@
         <v>5</v>
       </c>
       <c r="D13" s="3">
-        <f>(B13/$B$16)</f>
-        <v>0.10920695115361484</v>
+        <f t="shared" si="0"/>
+        <v>9.9736552996476421E-2</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19205,14 +19293,14 @@
         <v>7</v>
       </c>
       <c r="B14" s="2">
-        <v>147579</v>
+        <v>1553462</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="3">
-        <f>(B14/$B$16)</f>
-        <v>9.9675693834961176E-3</v>
+        <f t="shared" si="0"/>
+        <v>9.5822922063648758E-2</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19226,14 +19314,26 @@
         <v>6</v>
       </c>
       <c r="D15" s="3">
-        <f>(B15/$B$16)</f>
-        <v>0.12852969959677943</v>
+        <f t="shared" si="0"/>
+        <v>0.11738363776334639</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>33</v>
+      </c>
       <c r="B16" s="14">
         <f>SUM(B1:B15)</f>
-        <v>14805916.5</v>
+        <v>16211799.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="16">
+        <f>B16/B6</f>
+        <v>141.48273770563338</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -19403,7 +19503,7 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19423,8 +19523,8 @@
         <v>8</v>
       </c>
       <c r="D1" s="3">
-        <f>(B1/$B$16)</f>
-        <v>1.8151257303119332E-2</v>
+        <f t="shared" ref="D1:D15" si="0">(B1/$B$16)</f>
+        <v>1.6577185031186697E-2</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19438,8 +19538,8 @@
         <v>9</v>
       </c>
       <c r="D2" s="3">
-        <f>(B2/$B$16)</f>
-        <v>3.5309431874750878E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.2247407204857179E-2</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19453,8 +19553,8 @@
         <v>10</v>
       </c>
       <c r="D3" s="3">
-        <f>(B3/$B$16)</f>
-        <v>1.3147176670893693E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.200705695872935E-2</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19468,8 +19568,8 @@
         <v>0</v>
       </c>
       <c r="D4" s="3">
-        <f>(B4/$B$16)</f>
-        <v>4.5613657216019017E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.1658052827509985E-2</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19483,8 +19583,8 @@
         <v>1</v>
       </c>
       <c r="D5" s="3">
-        <f>(B5/$B$16)</f>
-        <v>0.18266346429820809</v>
+        <f t="shared" si="0"/>
+        <v>0.16682293659010525</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19496,8 +19596,8 @@
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="3">
-        <f>(B6/$B$16)</f>
-        <v>5.2531702444762541E-3</v>
+        <f t="shared" si="0"/>
+        <v>4.7976166988741749E-3</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19512,8 +19612,8 @@
         <v>2</v>
       </c>
       <c r="D7" s="3">
-        <f>(B7/$B$16)</f>
-        <v>0.1006604353063858</v>
+        <f t="shared" si="0"/>
+        <v>9.1931188761617738E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19527,8 +19627,8 @@
         <v>3</v>
       </c>
       <c r="D8" s="3">
-        <f>(B8/$B$16)</f>
-        <v>3.8492922744768961E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.5154826581712907E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19542,8 +19642,8 @@
         <v>11</v>
       </c>
       <c r="D9" s="3">
-        <f>(B9/$B$16)</f>
-        <v>0.12009408536107846</v>
+        <f t="shared" si="0"/>
+        <v>0.10967955778135549</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19557,8 +19657,8 @@
         <v>12</v>
       </c>
       <c r="D10" s="3">
-        <f>(B10/$B$16)</f>
-        <v>0.11695108506116457</v>
+        <f t="shared" si="0"/>
+        <v>0.1068091176429859</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19572,8 +19672,8 @@
         <v>14</v>
       </c>
       <c r="D11" s="3">
-        <f>(B11/$B$16)</f>
-        <v>4.3968909320811045E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.0155937038328163E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19587,8 +19687,8 @@
         <v>15</v>
       </c>
       <c r="D12" s="3">
-        <f>(B12/$B$16)</f>
-        <v>3.1990184464433524E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.92160040592656E-2</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19602,8 +19702,8 @@
         <v>5</v>
       </c>
       <c r="D13" s="3">
-        <f>(B13/$B$16)</f>
-        <v>0.10920695115361484</v>
+        <f t="shared" si="0"/>
+        <v>9.9736552996476421E-2</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19611,14 +19711,14 @@
         <v>7</v>
       </c>
       <c r="B14" s="2">
-        <v>147579</v>
+        <v>1553462</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="3">
-        <f>(B14/$B$16)</f>
-        <v>9.9675693834961176E-3</v>
+        <f t="shared" si="0"/>
+        <v>9.5822922063648758E-2</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19632,14 +19732,26 @@
         <v>6</v>
       </c>
       <c r="D15" s="3">
-        <f>(B15/$B$16)</f>
-        <v>0.12852969959677943</v>
+        <f t="shared" si="0"/>
+        <v>0.11738363776334639</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>33</v>
+      </c>
       <c r="B16" s="14">
         <f>SUM(B1:B15)</f>
-        <v>14805916.5</v>
+        <v>16211799.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="16">
+        <f>B16/B6</f>
+        <v>208.43682660906683</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -19809,7 +19921,7 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19829,8 +19941,8 @@
         <v>8</v>
       </c>
       <c r="D1" s="3">
-        <f>(B1/$B$16)</f>
-        <v>1.8151257303119332E-2</v>
+        <f t="shared" ref="D1:D15" si="0">(B1/$B$16)</f>
+        <v>1.6577185031186697E-2</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19844,8 +19956,8 @@
         <v>9</v>
       </c>
       <c r="D2" s="3">
-        <f>(B2/$B$16)</f>
-        <v>3.5309431874750878E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.2247407204857179E-2</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19859,8 +19971,8 @@
         <v>10</v>
       </c>
       <c r="D3" s="3">
-        <f>(B3/$B$16)</f>
-        <v>1.3147176670893693E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.200705695872935E-2</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19872,8 +19984,8 @@
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="3">
-        <f>(B4/$B$16)</f>
-        <v>7.2600031210496158E-3</v>
+        <f t="shared" si="0"/>
+        <v>6.6304175548186368E-3</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19888,8 +20000,8 @@
         <v>0</v>
       </c>
       <c r="D5" s="3">
-        <f>(B5/$B$16)</f>
-        <v>3.8353654094969401E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.502763527269135E-2</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19903,8 +20015,8 @@
         <v>1</v>
       </c>
       <c r="D6" s="3">
-        <f>(B6/$B$16)</f>
-        <v>0.18266346429820809</v>
+        <f t="shared" si="0"/>
+        <v>0.16682293659010525</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19918,8 +20030,8 @@
         <v>2</v>
       </c>
       <c r="D7" s="3">
-        <f>(B7/$B$16)</f>
-        <v>0.10591360555086204</v>
+        <f t="shared" si="0"/>
+        <v>9.672880546049191E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19933,8 +20045,8 @@
         <v>3</v>
       </c>
       <c r="D8" s="3">
-        <f>(B8/$B$16)</f>
-        <v>3.8492922744768961E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.5154826581712907E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19948,8 +20060,8 @@
         <v>11</v>
       </c>
       <c r="D9" s="3">
-        <f>(B9/$B$16)</f>
-        <v>0.12009408536107846</v>
+        <f t="shared" si="0"/>
+        <v>0.10967955778135549</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19963,8 +20075,8 @@
         <v>12</v>
       </c>
       <c r="D10" s="3">
-        <f>(B10/$B$16)</f>
-        <v>0.11695108506116457</v>
+        <f t="shared" si="0"/>
+        <v>0.1068091176429859</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19978,8 +20090,8 @@
         <v>14</v>
       </c>
       <c r="D11" s="3">
-        <f>(B11/$B$16)</f>
-        <v>4.3968909320811045E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.0155937038328163E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19993,8 +20105,8 @@
         <v>15</v>
       </c>
       <c r="D12" s="3">
-        <f>(B12/$B$16)</f>
-        <v>3.1990184464433524E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.92160040592656E-2</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -20008,8 +20120,8 @@
         <v>5</v>
       </c>
       <c r="D13" s="3">
-        <f>(B13/$B$16)</f>
-        <v>0.10920695115361484</v>
+        <f t="shared" si="0"/>
+        <v>9.9736552996476421E-2</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -20017,14 +20129,14 @@
         <v>7</v>
       </c>
       <c r="B14" s="2">
-        <v>147579</v>
+        <v>1553462</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="3">
-        <f>(B14/$B$16)</f>
-        <v>9.9675693834961176E-3</v>
+        <f t="shared" si="0"/>
+        <v>9.5822922063648758E-2</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -20038,14 +20150,26 @@
         <v>6</v>
       </c>
       <c r="D15" s="3">
-        <f>(B15/$B$16)</f>
-        <v>0.12852969959677943</v>
+        <f t="shared" si="0"/>
+        <v>0.11738363776334639</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16">
+      <c r="A16" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="14">
         <f>SUM(B1:B15)</f>
-        <v>14805916.5</v>
+        <v>16211799.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="16">
+        <f>B16/B4</f>
+        <v>150.82006400535857</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -20215,12 +20339,13 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="A16" sqref="A16:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="9" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -20235,8 +20360,8 @@
         <v>8</v>
       </c>
       <c r="D1" s="3">
-        <f>(B1/$B$16)</f>
-        <v>1.8151257303119332E-2</v>
+        <f t="shared" ref="D1:D15" si="0">(B1/$B$16)</f>
+        <v>1.6577185031186697E-2</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -20250,8 +20375,8 @@
         <v>9</v>
       </c>
       <c r="D2" s="3">
-        <f>(B2/$B$16)</f>
-        <v>3.5309431874750878E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.2247407204857179E-2</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -20265,8 +20390,8 @@
         <v>10</v>
       </c>
       <c r="D3" s="3">
-        <f>(B3/$B$16)</f>
-        <v>1.3147176670893693E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.200705695872935E-2</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -20278,8 +20403,8 @@
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="3">
-        <f>(B4/$B$16)</f>
-        <v>9.4652701843887885E-3</v>
+        <f t="shared" si="0"/>
+        <v>8.6444444369053533E-3</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -20294,8 +20419,8 @@
         <v>0</v>
       </c>
       <c r="D5" s="3">
-        <f>(B5/$B$16)</f>
-        <v>3.614838703163023E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.3013608390604632E-2</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -20309,8 +20434,8 @@
         <v>1</v>
       </c>
       <c r="D6" s="3">
-        <f>(B6/$B$16)</f>
-        <v>0.18266346429820809</v>
+        <f t="shared" si="0"/>
+        <v>0.16682293659010525</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -20324,8 +20449,8 @@
         <v>2</v>
       </c>
       <c r="D7" s="3">
-        <f>(B7/$B$16)</f>
-        <v>0.10591360555086204</v>
+        <f t="shared" si="0"/>
+        <v>9.672880546049191E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -20339,8 +20464,8 @@
         <v>3</v>
       </c>
       <c r="D8" s="3">
-        <f>(B8/$B$16)</f>
-        <v>3.8492922744768961E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.5154826581712907E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -20354,8 +20479,8 @@
         <v>11</v>
       </c>
       <c r="D9" s="3">
-        <f>(B9/$B$16)</f>
-        <v>0.12009408536107846</v>
+        <f t="shared" si="0"/>
+        <v>0.10967955778135549</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -20369,8 +20494,8 @@
         <v>12</v>
       </c>
       <c r="D10" s="3">
-        <f>(B10/$B$16)</f>
-        <v>0.11695108506116457</v>
+        <f t="shared" si="0"/>
+        <v>0.1068091176429859</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -20384,8 +20509,8 @@
         <v>14</v>
       </c>
       <c r="D11" s="3">
-        <f>(B11/$B$16)</f>
-        <v>4.3968909320811045E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.0155937038328163E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -20399,8 +20524,8 @@
         <v>15</v>
       </c>
       <c r="D12" s="3">
-        <f>(B12/$B$16)</f>
-        <v>3.1990184464433524E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.92160040592656E-2</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -20414,8 +20539,8 @@
         <v>5</v>
       </c>
       <c r="D13" s="3">
-        <f>(B13/$B$16)</f>
-        <v>0.10920695115361484</v>
+        <f t="shared" si="0"/>
+        <v>9.9736552996476421E-2</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -20423,14 +20548,14 @@
         <v>7</v>
       </c>
       <c r="B14" s="2">
-        <v>147579</v>
+        <v>1553462</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="3">
-        <f>(B14/$B$16)</f>
-        <v>9.9675693834961176E-3</v>
+        <f t="shared" si="0"/>
+        <v>9.5822922063648758E-2</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -20444,14 +20569,26 @@
         <v>6</v>
       </c>
       <c r="D15" s="3">
-        <f>(B15/$B$16)</f>
-        <v>0.12852969959677943</v>
+        <f t="shared" si="0"/>
+        <v>0.11738363776334639</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>33</v>
+      </c>
       <c r="B16" s="14">
         <f>SUM(B1:B15)</f>
-        <v>14805916.5</v>
+        <v>16211799.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="16">
+        <f>B16/B4</f>
+        <v>115.68123403405117</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>